<commit_message>
run all scenario sulawesi selatan
</commit_message>
<xml_diff>
--- a/_DB/data/SumSel/Building LDMProp and LUTM template.xlsx
+++ b/_DB/data/SumSel/Building LDMProp and LUTM template.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\icrafguest01\tin\pprk_apps_tinbaru\aksara_rancang\_DB\data\SumSel\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D266C785-74EB-40ED-A1E5-92E711605F71}" xr6:coauthVersionLast="44" xr6:coauthVersionMax="44" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2CC0F356-E438-45A3-9F1B-2F862F7BB6B3}" xr6:coauthVersionLast="44" xr6:coauthVersionMax="44" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -5866,15 +5866,18 @@
   <dimension ref="A1:Y63"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="G1" workbookViewId="0">
-      <selection activeCell="O3" sqref="O3"/>
+      <selection activeCell="B62" sqref="B1:X62"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="21.42578125" customWidth="1"/>
+    <col min="1" max="1" width="29.42578125" customWidth="1"/>
     <col min="3" max="3" width="12.28515625" customWidth="1"/>
     <col min="5" max="5" width="12.5703125" customWidth="1"/>
     <col min="6" max="6" width="14.85546875" customWidth="1"/>
+    <col min="7" max="7" width="11.7109375" customWidth="1"/>
+    <col min="11" max="11" width="9.5703125" customWidth="1"/>
+    <col min="13" max="13" width="11.85546875" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:25" x14ac:dyDescent="0.25">
@@ -5980,7 +5983,7 @@
         <v>0</v>
       </c>
       <c r="K2">
-        <v>0.1</v>
+        <v>0.05</v>
       </c>
       <c r="L2">
         <v>0</v>
@@ -5992,7 +5995,7 @@
         <v>0</v>
       </c>
       <c r="O2">
-        <v>8.9999999999999993E-3</v>
+        <v>0.999</v>
       </c>
       <c r="P2">
         <v>0</v>
@@ -6013,7 +6016,7 @@
         <v>0</v>
       </c>
       <c r="V2">
-        <v>0.1</v>
+        <v>0.03</v>
       </c>
       <c r="W2">
         <v>0</v>
@@ -6023,7 +6026,7 @@
       </c>
       <c r="Y2">
         <f>SUM(B2:X2)</f>
-        <v>0.20900000000000002</v>
+        <v>1.079</v>
       </c>
     </row>
     <row r="3" spans="1:25" x14ac:dyDescent="0.25">
@@ -6064,7 +6067,7 @@
         <v>0</v>
       </c>
       <c r="M3">
-        <v>0.1</v>
+        <v>0.2</v>
       </c>
       <c r="N3">
         <v>0</v>
@@ -6079,7 +6082,7 @@
         <v>0</v>
       </c>
       <c r="R3">
-        <v>0.1</v>
+        <v>0.05</v>
       </c>
       <c r="S3">
         <v>0</v>
@@ -6101,7 +6104,7 @@
       </c>
       <c r="Y3">
         <f t="shared" ref="Y3:Y62" si="0">SUM(B3:X3)</f>
-        <v>0.2</v>
+        <v>0.25</v>
       </c>
     </row>
     <row r="4" spans="1:25" x14ac:dyDescent="0.25">
@@ -6142,7 +6145,7 @@
         <v>0</v>
       </c>
       <c r="M4">
-        <v>0.1</v>
+        <v>0.2</v>
       </c>
       <c r="N4">
         <v>0</v>
@@ -6157,7 +6160,7 @@
         <v>0</v>
       </c>
       <c r="R4">
-        <v>0.1</v>
+        <v>0.05</v>
       </c>
       <c r="S4">
         <v>0</v>
@@ -6179,7 +6182,7 @@
       </c>
       <c r="Y4">
         <f t="shared" si="0"/>
-        <v>0.2</v>
+        <v>0.25</v>
       </c>
     </row>
     <row r="5" spans="1:25" x14ac:dyDescent="0.25">
@@ -6220,7 +6223,7 @@
         <v>0</v>
       </c>
       <c r="M5">
-        <v>0.1</v>
+        <v>0.2</v>
       </c>
       <c r="N5">
         <v>0</v>
@@ -6235,7 +6238,7 @@
         <v>0</v>
       </c>
       <c r="R5">
-        <v>0.1</v>
+        <v>0.05</v>
       </c>
       <c r="S5">
         <v>0</v>
@@ -6257,7 +6260,7 @@
       </c>
       <c r="Y5">
         <f t="shared" si="0"/>
-        <v>0.2</v>
+        <v>0.25</v>
       </c>
     </row>
     <row r="6" spans="1:25" x14ac:dyDescent="0.25">
@@ -6298,7 +6301,7 @@
         <v>0</v>
       </c>
       <c r="M6">
-        <v>0.1</v>
+        <v>0.2</v>
       </c>
       <c r="N6">
         <v>0</v>
@@ -6313,7 +6316,7 @@
         <v>0</v>
       </c>
       <c r="R6">
-        <v>0.1</v>
+        <v>0.05</v>
       </c>
       <c r="S6">
         <v>0</v>
@@ -6335,7 +6338,7 @@
       </c>
       <c r="Y6">
         <f t="shared" si="0"/>
-        <v>0.2</v>
+        <v>0.25</v>
       </c>
     </row>
     <row r="7" spans="1:25" x14ac:dyDescent="0.25">
@@ -6391,7 +6394,7 @@
         <v>0</v>
       </c>
       <c r="R7">
-        <v>0.1</v>
+        <v>0.05</v>
       </c>
       <c r="S7">
         <v>0</v>
@@ -6413,7 +6416,7 @@
       </c>
       <c r="Y7">
         <f t="shared" si="0"/>
-        <v>0.30000000000000004</v>
+        <v>0.25</v>
       </c>
     </row>
     <row r="8" spans="1:25" x14ac:dyDescent="0.25">
@@ -6469,7 +6472,7 @@
         <v>0</v>
       </c>
       <c r="R8">
-        <v>0.1</v>
+        <v>0.05</v>
       </c>
       <c r="S8">
         <v>0</v>
@@ -6491,7 +6494,7 @@
       </c>
       <c r="Y8">
         <f t="shared" si="0"/>
-        <v>0.30000000000000004</v>
+        <v>0.25</v>
       </c>
     </row>
     <row r="9" spans="1:25" x14ac:dyDescent="0.25">
@@ -6547,7 +6550,7 @@
         <v>0</v>
       </c>
       <c r="R9">
-        <v>0.1</v>
+        <v>0.05</v>
       </c>
       <c r="S9">
         <v>0</v>
@@ -6569,7 +6572,7 @@
       </c>
       <c r="Y9">
         <f t="shared" si="0"/>
-        <v>0.30000000000000004</v>
+        <v>0.25</v>
       </c>
     </row>
     <row r="10" spans="1:25" x14ac:dyDescent="0.25">
@@ -6613,7 +6616,8 @@
         <v>0</v>
       </c>
       <c r="N10">
-        <v>0.1</v>
+        <f>1-0.701</f>
+        <v>0.29900000000000004</v>
       </c>
       <c r="O10">
         <v>0</v>
@@ -6625,7 +6629,7 @@
         <v>0</v>
       </c>
       <c r="R10">
-        <v>0.1</v>
+        <v>0.05</v>
       </c>
       <c r="S10">
         <v>0</v>
@@ -6647,7 +6651,7 @@
       </c>
       <c r="Y10">
         <f t="shared" si="0"/>
-        <v>0.5</v>
+        <v>0.64900000000000002</v>
       </c>
     </row>
     <row r="11" spans="1:25" x14ac:dyDescent="0.25">
@@ -6922,7 +6926,7 @@
         <v>0</v>
       </c>
       <c r="M14">
-        <v>0</v>
+        <v>0.2</v>
       </c>
       <c r="N14">
         <v>0.1</v>
@@ -6959,7 +6963,7 @@
       </c>
       <c r="Y14">
         <f t="shared" si="0"/>
-        <v>0.4</v>
+        <v>0.6</v>
       </c>
     </row>
     <row r="15" spans="1:25" x14ac:dyDescent="0.25">
@@ -6991,13 +6995,13 @@
         <v>0</v>
       </c>
       <c r="J15">
-        <v>0</v>
+        <v>0.15</v>
       </c>
       <c r="K15">
         <v>0</v>
       </c>
       <c r="L15">
-        <v>0.2</v>
+        <v>0.25</v>
       </c>
       <c r="M15">
         <v>0</v>
@@ -7037,7 +7041,7 @@
       </c>
       <c r="Y15">
         <f t="shared" si="0"/>
-        <v>0.2</v>
+        <v>0.4</v>
       </c>
     </row>
     <row r="16" spans="1:25" x14ac:dyDescent="0.25">
@@ -7090,8 +7094,8 @@
         <v>0</v>
       </c>
       <c r="Q16">
-        <f>0.3/39</f>
-        <v>7.6923076923076919E-3</v>
+        <f t="shared" ref="Q16:Q17" si="1">0.2/39</f>
+        <v>5.1282051282051282E-3</v>
       </c>
       <c r="R16">
         <v>0</v>
@@ -7116,7 +7120,7 @@
       </c>
       <c r="Y16">
         <f t="shared" si="0"/>
-        <v>7.6923076923076919E-3</v>
+        <v>5.1282051282051282E-3</v>
       </c>
     </row>
     <row r="17" spans="1:25" x14ac:dyDescent="0.25">
@@ -7169,8 +7173,8 @@
         <v>0</v>
       </c>
       <c r="Q17">
-        <f>0.3/39</f>
-        <v>7.6923076923076919E-3</v>
+        <f t="shared" si="1"/>
+        <v>5.1282051282051282E-3</v>
       </c>
       <c r="R17">
         <v>0</v>
@@ -7195,7 +7199,7 @@
       </c>
       <c r="Y17">
         <f t="shared" si="0"/>
-        <v>7.6923076923076919E-3</v>
+        <v>5.1282051282051282E-3</v>
       </c>
     </row>
     <row r="18" spans="1:25" x14ac:dyDescent="0.25">
@@ -7203,34 +7207,34 @@
         <v>92</v>
       </c>
       <c r="B18">
-        <v>0.1</v>
+        <v>0.2</v>
       </c>
       <c r="C18">
         <v>0.3</v>
       </c>
       <c r="D18">
-        <v>0.1</v>
+        <v>0</v>
       </c>
       <c r="E18">
+        <v>0.3</v>
+      </c>
+      <c r="F18">
         <v>0.2</v>
       </c>
-      <c r="F18">
-        <v>0.1</v>
-      </c>
       <c r="G18">
-        <v>0.1</v>
+        <v>0.2</v>
       </c>
       <c r="H18">
-        <v>0.8</v>
+        <v>0.9</v>
       </c>
       <c r="I18">
         <v>0</v>
       </c>
       <c r="J18">
-        <v>0.1</v>
+        <v>0</v>
       </c>
       <c r="K18">
-        <v>0.1</v>
+        <v>0</v>
       </c>
       <c r="L18">
         <v>0</v>
@@ -7263,7 +7267,7 @@
         <v>0</v>
       </c>
       <c r="V18">
-        <v>0.1</v>
+        <v>0</v>
       </c>
       <c r="W18">
         <v>0</v>
@@ -7273,7 +7277,7 @@
       </c>
       <c r="Y18">
         <f t="shared" si="0"/>
-        <v>2</v>
+        <v>2.1</v>
       </c>
     </row>
     <row r="19" spans="1:25" x14ac:dyDescent="0.25">
@@ -7293,10 +7297,10 @@
         <v>0</v>
       </c>
       <c r="F19">
-        <v>0</v>
+        <v>0.2</v>
       </c>
       <c r="G19">
-        <v>0</v>
+        <v>0.2</v>
       </c>
       <c r="H19">
         <v>0</v>
@@ -7323,7 +7327,7 @@
         <v>0</v>
       </c>
       <c r="P19">
-        <v>0.6</v>
+        <v>0.55000000000000004</v>
       </c>
       <c r="Q19">
         <v>0</v>
@@ -7338,10 +7342,10 @@
         <v>0</v>
       </c>
       <c r="U19">
-        <v>0.6</v>
+        <v>0.3</v>
       </c>
       <c r="V19">
-        <v>0</v>
+        <v>0.01</v>
       </c>
       <c r="W19">
         <v>0</v>
@@ -7351,7 +7355,7 @@
       </c>
       <c r="Y19">
         <f t="shared" si="0"/>
-        <v>1.2</v>
+        <v>1.26</v>
       </c>
     </row>
     <row r="20" spans="1:25" x14ac:dyDescent="0.25">
@@ -7410,7 +7414,7 @@
         <v>0</v>
       </c>
       <c r="S20">
-        <v>0.1</v>
+        <v>0.05</v>
       </c>
       <c r="T20">
         <v>0.4</v>
@@ -7429,7 +7433,7 @@
       </c>
       <c r="Y20">
         <f t="shared" si="0"/>
-        <v>0.5</v>
+        <v>0.45</v>
       </c>
     </row>
     <row r="21" spans="1:25" x14ac:dyDescent="0.25">
@@ -7488,7 +7492,7 @@
         <v>0</v>
       </c>
       <c r="S21">
-        <v>0.1</v>
+        <v>0.05</v>
       </c>
       <c r="T21">
         <v>0.2</v>
@@ -7507,7 +7511,7 @@
       </c>
       <c r="Y21">
         <f t="shared" si="0"/>
-        <v>0.30000000000000004</v>
+        <v>0.25</v>
       </c>
     </row>
     <row r="22" spans="1:25" x14ac:dyDescent="0.25">
@@ -7566,7 +7570,7 @@
         <v>0</v>
       </c>
       <c r="S22">
-        <v>0.2</v>
+        <v>0.05</v>
       </c>
       <c r="T22">
         <v>0.2</v>
@@ -7585,7 +7589,7 @@
       </c>
       <c r="Y22">
         <f t="shared" si="0"/>
-        <v>0.4</v>
+        <v>0.25</v>
       </c>
     </row>
     <row r="23" spans="1:25" x14ac:dyDescent="0.25">
@@ -7644,7 +7648,7 @@
         <v>0</v>
       </c>
       <c r="S23">
-        <v>0.2</v>
+        <v>0.05</v>
       </c>
       <c r="T23">
         <v>0.2</v>
@@ -7663,7 +7667,7 @@
       </c>
       <c r="Y23">
         <f t="shared" si="0"/>
-        <v>0.4</v>
+        <v>0.25</v>
       </c>
     </row>
     <row r="24" spans="1:25" x14ac:dyDescent="0.25">
@@ -7716,8 +7720,8 @@
         <v>0</v>
       </c>
       <c r="Q24">
-        <f>0.3/39</f>
-        <v>7.6923076923076919E-3</v>
+        <f>0.2/39</f>
+        <v>5.1282051282051282E-3</v>
       </c>
       <c r="R24">
         <v>0</v>
@@ -7742,7 +7746,7 @@
       </c>
       <c r="Y24">
         <f t="shared" si="0"/>
-        <v>7.6923076923076919E-3</v>
+        <v>5.1282051282051282E-3</v>
       </c>
     </row>
     <row r="25" spans="1:25" x14ac:dyDescent="0.25">
@@ -7795,8 +7799,8 @@
         <v>0</v>
       </c>
       <c r="Q25">
-        <f t="shared" ref="Q25:Q60" si="1">0.3/39</f>
-        <v>7.6923076923076919E-3</v>
+        <f t="shared" ref="Q25:Q60" si="2">0.2/39</f>
+        <v>5.1282051282051282E-3</v>
       </c>
       <c r="R25">
         <v>0</v>
@@ -7821,7 +7825,7 @@
       </c>
       <c r="Y25">
         <f t="shared" si="0"/>
-        <v>7.6923076923076919E-3</v>
+        <v>5.1282051282051282E-3</v>
       </c>
     </row>
     <row r="26" spans="1:25" x14ac:dyDescent="0.25">
@@ -7874,8 +7878,8 @@
         <v>0</v>
       </c>
       <c r="Q26">
-        <f t="shared" si="1"/>
-        <v>7.6923076923076919E-3</v>
+        <f t="shared" si="2"/>
+        <v>5.1282051282051282E-3</v>
       </c>
       <c r="R26">
         <v>0</v>
@@ -7900,7 +7904,7 @@
       </c>
       <c r="Y26">
         <f t="shared" si="0"/>
-        <v>7.6923076923076919E-3</v>
+        <v>5.1282051282051282E-3</v>
       </c>
     </row>
     <row r="27" spans="1:25" x14ac:dyDescent="0.25">
@@ -7953,8 +7957,8 @@
         <v>0</v>
       </c>
       <c r="Q27">
-        <f t="shared" si="1"/>
-        <v>7.6923076923076919E-3</v>
+        <f t="shared" si="2"/>
+        <v>5.1282051282051282E-3</v>
       </c>
       <c r="R27">
         <v>0</v>
@@ -7979,7 +7983,7 @@
       </c>
       <c r="Y27">
         <f t="shared" si="0"/>
-        <v>7.6923076923076919E-3</v>
+        <v>5.1282051282051282E-3</v>
       </c>
     </row>
     <row r="28" spans="1:25" x14ac:dyDescent="0.25">
@@ -8032,8 +8036,8 @@
         <v>0</v>
       </c>
       <c r="Q28">
-        <f t="shared" si="1"/>
-        <v>7.6923076923076919E-3</v>
+        <f t="shared" si="2"/>
+        <v>5.1282051282051282E-3</v>
       </c>
       <c r="R28">
         <v>0</v>
@@ -8058,7 +8062,7 @@
       </c>
       <c r="Y28">
         <f t="shared" si="0"/>
-        <v>7.6923076923076919E-3</v>
+        <v>5.1282051282051282E-3</v>
       </c>
     </row>
     <row r="29" spans="1:25" x14ac:dyDescent="0.25">
@@ -8111,8 +8115,8 @@
         <v>0</v>
       </c>
       <c r="Q29">
-        <f t="shared" si="1"/>
-        <v>7.6923076923076919E-3</v>
+        <f t="shared" si="2"/>
+        <v>5.1282051282051282E-3</v>
       </c>
       <c r="R29">
         <v>0</v>
@@ -8137,7 +8141,7 @@
       </c>
       <c r="Y29">
         <f t="shared" si="0"/>
-        <v>7.6923076923076919E-3</v>
+        <v>5.1282051282051282E-3</v>
       </c>
     </row>
     <row r="30" spans="1:25" x14ac:dyDescent="0.25">
@@ -8190,8 +8194,8 @@
         <v>0</v>
       </c>
       <c r="Q30">
-        <f t="shared" si="1"/>
-        <v>7.6923076923076919E-3</v>
+        <f t="shared" si="2"/>
+        <v>5.1282051282051282E-3</v>
       </c>
       <c r="R30">
         <v>0</v>
@@ -8216,7 +8220,7 @@
       </c>
       <c r="Y30">
         <f t="shared" si="0"/>
-        <v>7.6923076923076919E-3</v>
+        <v>5.1282051282051282E-3</v>
       </c>
     </row>
     <row r="31" spans="1:25" x14ac:dyDescent="0.25">
@@ -8269,8 +8273,8 @@
         <v>0</v>
       </c>
       <c r="Q31">
-        <f t="shared" si="1"/>
-        <v>7.6923076923076919E-3</v>
+        <f t="shared" si="2"/>
+        <v>5.1282051282051282E-3</v>
       </c>
       <c r="R31">
         <v>0</v>
@@ -8295,7 +8299,7 @@
       </c>
       <c r="Y31">
         <f t="shared" si="0"/>
-        <v>7.6923076923076919E-3</v>
+        <v>5.1282051282051282E-3</v>
       </c>
     </row>
     <row r="32" spans="1:25" x14ac:dyDescent="0.25">
@@ -8348,8 +8352,8 @@
         <v>0</v>
       </c>
       <c r="Q32">
-        <f t="shared" si="1"/>
-        <v>7.6923076923076919E-3</v>
+        <f t="shared" si="2"/>
+        <v>5.1282051282051282E-3</v>
       </c>
       <c r="R32">
         <v>0</v>
@@ -8374,7 +8378,7 @@
       </c>
       <c r="Y32">
         <f t="shared" si="0"/>
-        <v>7.6923076923076919E-3</v>
+        <v>5.1282051282051282E-3</v>
       </c>
     </row>
     <row r="33" spans="1:25" x14ac:dyDescent="0.25">
@@ -8427,8 +8431,8 @@
         <v>0</v>
       </c>
       <c r="Q33">
-        <f t="shared" si="1"/>
-        <v>7.6923076923076919E-3</v>
+        <f t="shared" si="2"/>
+        <v>5.1282051282051282E-3</v>
       </c>
       <c r="R33">
         <v>0</v>
@@ -8453,7 +8457,7 @@
       </c>
       <c r="Y33">
         <f t="shared" si="0"/>
-        <v>7.6923076923076919E-3</v>
+        <v>5.1282051282051282E-3</v>
       </c>
     </row>
     <row r="34" spans="1:25" x14ac:dyDescent="0.25">
@@ -8506,8 +8510,8 @@
         <v>0</v>
       </c>
       <c r="Q34">
-        <f t="shared" si="1"/>
-        <v>7.6923076923076919E-3</v>
+        <f t="shared" si="2"/>
+        <v>5.1282051282051282E-3</v>
       </c>
       <c r="R34">
         <v>0</v>
@@ -8532,7 +8536,7 @@
       </c>
       <c r="Y34">
         <f t="shared" si="0"/>
-        <v>7.6923076923076919E-3</v>
+        <v>5.1282051282051282E-3</v>
       </c>
     </row>
     <row r="35" spans="1:25" x14ac:dyDescent="0.25">
@@ -8585,8 +8589,8 @@
         <v>0</v>
       </c>
       <c r="Q35">
-        <f t="shared" si="1"/>
-        <v>7.6923076923076919E-3</v>
+        <f t="shared" si="2"/>
+        <v>5.1282051282051282E-3</v>
       </c>
       <c r="R35">
         <v>0</v>
@@ -8611,7 +8615,7 @@
       </c>
       <c r="Y35">
         <f t="shared" si="0"/>
-        <v>7.6923076923076919E-3</v>
+        <v>5.1282051282051282E-3</v>
       </c>
     </row>
     <row r="36" spans="1:25" x14ac:dyDescent="0.25">
@@ -8664,8 +8668,8 @@
         <v>0</v>
       </c>
       <c r="Q36">
-        <f t="shared" si="1"/>
-        <v>7.6923076923076919E-3</v>
+        <f t="shared" si="2"/>
+        <v>5.1282051282051282E-3</v>
       </c>
       <c r="R36">
         <v>0</v>
@@ -8690,7 +8694,7 @@
       </c>
       <c r="Y36">
         <f t="shared" si="0"/>
-        <v>7.6923076923076919E-3</v>
+        <v>5.1282051282051282E-3</v>
       </c>
     </row>
     <row r="37" spans="1:25" x14ac:dyDescent="0.25">
@@ -8743,8 +8747,8 @@
         <v>0</v>
       </c>
       <c r="Q37">
-        <f t="shared" si="1"/>
-        <v>7.6923076923076919E-3</v>
+        <f t="shared" si="2"/>
+        <v>5.1282051282051282E-3</v>
       </c>
       <c r="R37">
         <v>0</v>
@@ -8769,7 +8773,7 @@
       </c>
       <c r="Y37">
         <f t="shared" si="0"/>
-        <v>7.6923076923076919E-3</v>
+        <v>5.1282051282051282E-3</v>
       </c>
     </row>
     <row r="38" spans="1:25" x14ac:dyDescent="0.25">
@@ -8822,8 +8826,8 @@
         <v>0</v>
       </c>
       <c r="Q38">
-        <f t="shared" si="1"/>
-        <v>7.6923076923076919E-3</v>
+        <f t="shared" si="2"/>
+        <v>5.1282051282051282E-3</v>
       </c>
       <c r="R38">
         <v>0</v>
@@ -8848,7 +8852,7 @@
       </c>
       <c r="Y38">
         <f t="shared" si="0"/>
-        <v>7.6923076923076919E-3</v>
+        <v>5.1282051282051282E-3</v>
       </c>
     </row>
     <row r="39" spans="1:25" x14ac:dyDescent="0.25">
@@ -8901,8 +8905,8 @@
         <v>0</v>
       </c>
       <c r="Q39">
-        <f t="shared" si="1"/>
-        <v>7.6923076923076919E-3</v>
+        <f t="shared" si="2"/>
+        <v>5.1282051282051282E-3</v>
       </c>
       <c r="R39">
         <v>0</v>
@@ -8927,7 +8931,7 @@
       </c>
       <c r="Y39">
         <f t="shared" si="0"/>
-        <v>7.6923076923076919E-3</v>
+        <v>5.1282051282051282E-3</v>
       </c>
     </row>
     <row r="40" spans="1:25" x14ac:dyDescent="0.25">
@@ -8980,8 +8984,8 @@
         <v>0</v>
       </c>
       <c r="Q40">
-        <f t="shared" si="1"/>
-        <v>7.6923076923076919E-3</v>
+        <f t="shared" si="2"/>
+        <v>5.1282051282051282E-3</v>
       </c>
       <c r="R40">
         <v>0</v>
@@ -9006,7 +9010,7 @@
       </c>
       <c r="Y40">
         <f t="shared" si="0"/>
-        <v>7.6923076923076919E-3</v>
+        <v>5.1282051282051282E-3</v>
       </c>
     </row>
     <row r="41" spans="1:25" x14ac:dyDescent="0.25">
@@ -9059,8 +9063,8 @@
         <v>0</v>
       </c>
       <c r="Q41">
-        <f t="shared" si="1"/>
-        <v>7.6923076923076919E-3</v>
+        <f t="shared" si="2"/>
+        <v>5.1282051282051282E-3</v>
       </c>
       <c r="R41">
         <v>0</v>
@@ -9085,7 +9089,7 @@
       </c>
       <c r="Y41">
         <f t="shared" si="0"/>
-        <v>7.6923076923076919E-3</v>
+        <v>5.1282051282051282E-3</v>
       </c>
     </row>
     <row r="42" spans="1:25" x14ac:dyDescent="0.25">
@@ -9138,8 +9142,8 @@
         <v>0</v>
       </c>
       <c r="Q42">
-        <f t="shared" si="1"/>
-        <v>7.6923076923076919E-3</v>
+        <f t="shared" si="2"/>
+        <v>5.1282051282051282E-3</v>
       </c>
       <c r="R42">
         <v>0</v>
@@ -9164,7 +9168,7 @@
       </c>
       <c r="Y42">
         <f t="shared" si="0"/>
-        <v>7.6923076923076919E-3</v>
+        <v>5.1282051282051282E-3</v>
       </c>
     </row>
     <row r="43" spans="1:25" x14ac:dyDescent="0.25">
@@ -9217,8 +9221,8 @@
         <v>0</v>
       </c>
       <c r="Q43">
-        <f t="shared" si="1"/>
-        <v>7.6923076923076919E-3</v>
+        <f t="shared" si="2"/>
+        <v>5.1282051282051282E-3</v>
       </c>
       <c r="R43">
         <v>0</v>
@@ -9243,7 +9247,7 @@
       </c>
       <c r="Y43">
         <f t="shared" si="0"/>
-        <v>7.6923076923076919E-3</v>
+        <v>5.1282051282051282E-3</v>
       </c>
     </row>
     <row r="44" spans="1:25" x14ac:dyDescent="0.25">
@@ -9296,8 +9300,8 @@
         <v>0</v>
       </c>
       <c r="Q44">
-        <f t="shared" si="1"/>
-        <v>7.6923076923076919E-3</v>
+        <f t="shared" si="2"/>
+        <v>5.1282051282051282E-3</v>
       </c>
       <c r="R44">
         <v>0</v>
@@ -9322,7 +9326,7 @@
       </c>
       <c r="Y44">
         <f t="shared" si="0"/>
-        <v>7.6923076923076919E-3</v>
+        <v>5.1282051282051282E-3</v>
       </c>
     </row>
     <row r="45" spans="1:25" x14ac:dyDescent="0.25">
@@ -9375,8 +9379,8 @@
         <v>0</v>
       </c>
       <c r="Q45">
-        <f t="shared" si="1"/>
-        <v>7.6923076923076919E-3</v>
+        <f t="shared" si="2"/>
+        <v>5.1282051282051282E-3</v>
       </c>
       <c r="R45">
         <v>0</v>
@@ -9401,7 +9405,7 @@
       </c>
       <c r="Y45">
         <f t="shared" si="0"/>
-        <v>7.6923076923076919E-3</v>
+        <v>5.1282051282051282E-3</v>
       </c>
     </row>
     <row r="46" spans="1:25" x14ac:dyDescent="0.25">
@@ -9454,8 +9458,8 @@
         <v>0</v>
       </c>
       <c r="Q46">
-        <f t="shared" si="1"/>
-        <v>7.6923076923076919E-3</v>
+        <f t="shared" si="2"/>
+        <v>5.1282051282051282E-3</v>
       </c>
       <c r="R46">
         <v>0</v>
@@ -9480,7 +9484,7 @@
       </c>
       <c r="Y46">
         <f t="shared" si="0"/>
-        <v>7.6923076923076919E-3</v>
+        <v>5.1282051282051282E-3</v>
       </c>
     </row>
     <row r="47" spans="1:25" x14ac:dyDescent="0.25">
@@ -9533,8 +9537,8 @@
         <v>0</v>
       </c>
       <c r="Q47">
-        <f t="shared" si="1"/>
-        <v>7.6923076923076919E-3</v>
+        <f t="shared" si="2"/>
+        <v>5.1282051282051282E-3</v>
       </c>
       <c r="R47">
         <v>0</v>
@@ -9559,7 +9563,7 @@
       </c>
       <c r="Y47">
         <f t="shared" si="0"/>
-        <v>7.6923076923076919E-3</v>
+        <v>5.1282051282051282E-3</v>
       </c>
     </row>
     <row r="48" spans="1:25" x14ac:dyDescent="0.25">
@@ -9612,8 +9616,8 @@
         <v>0</v>
       </c>
       <c r="Q48">
-        <f t="shared" si="1"/>
-        <v>7.6923076923076919E-3</v>
+        <f t="shared" si="2"/>
+        <v>5.1282051282051282E-3</v>
       </c>
       <c r="R48">
         <v>0</v>
@@ -9634,11 +9638,11 @@
         <v>0</v>
       </c>
       <c r="X48">
-        <v>0.2</v>
+        <v>0</v>
       </c>
       <c r="Y48">
         <f t="shared" si="0"/>
-        <v>0.2076923076923077</v>
+        <v>5.1282051282051282E-3</v>
       </c>
     </row>
     <row r="49" spans="1:25" x14ac:dyDescent="0.25">
@@ -9691,8 +9695,8 @@
         <v>0</v>
       </c>
       <c r="Q49">
-        <f t="shared" si="1"/>
-        <v>7.6923076923076919E-3</v>
+        <f t="shared" si="2"/>
+        <v>5.1282051282051282E-3</v>
       </c>
       <c r="R49">
         <v>0</v>
@@ -9717,7 +9721,7 @@
       </c>
       <c r="Y49">
         <f t="shared" si="0"/>
-        <v>7.6923076923076919E-3</v>
+        <v>5.1282051282051282E-3</v>
       </c>
     </row>
     <row r="50" spans="1:25" x14ac:dyDescent="0.25">
@@ -9770,8 +9774,8 @@
         <v>0</v>
       </c>
       <c r="Q50">
-        <f t="shared" si="1"/>
-        <v>7.6923076923076919E-3</v>
+        <f t="shared" si="2"/>
+        <v>5.1282051282051282E-3</v>
       </c>
       <c r="R50">
         <v>0</v>
@@ -9796,7 +9800,7 @@
       </c>
       <c r="Y50">
         <f t="shared" si="0"/>
-        <v>7.6923076923076919E-3</v>
+        <v>5.1282051282051282E-3</v>
       </c>
     </row>
     <row r="51" spans="1:25" x14ac:dyDescent="0.25">
@@ -9849,8 +9853,8 @@
         <v>0</v>
       </c>
       <c r="Q51">
-        <f t="shared" si="1"/>
-        <v>7.6923076923076919E-3</v>
+        <f t="shared" si="2"/>
+        <v>5.1282051282051282E-3</v>
       </c>
       <c r="R51">
         <v>0</v>
@@ -9875,7 +9879,7 @@
       </c>
       <c r="Y51">
         <f t="shared" si="0"/>
-        <v>7.6923076923076919E-3</v>
+        <v>5.1282051282051282E-3</v>
       </c>
     </row>
     <row r="52" spans="1:25" x14ac:dyDescent="0.25">
@@ -9928,8 +9932,8 @@
         <v>0</v>
       </c>
       <c r="Q52">
-        <f t="shared" si="1"/>
-        <v>7.6923076923076919E-3</v>
+        <f t="shared" si="2"/>
+        <v>5.1282051282051282E-3</v>
       </c>
       <c r="R52">
         <v>0</v>
@@ -9954,7 +9958,7 @@
       </c>
       <c r="Y52">
         <f t="shared" si="0"/>
-        <v>7.6923076923076919E-3</v>
+        <v>5.1282051282051282E-3</v>
       </c>
     </row>
     <row r="53" spans="1:25" x14ac:dyDescent="0.25">
@@ -10007,8 +10011,8 @@
         <v>0</v>
       </c>
       <c r="Q53">
-        <f t="shared" si="1"/>
-        <v>7.6923076923076919E-3</v>
+        <f t="shared" si="2"/>
+        <v>5.1282051282051282E-3</v>
       </c>
       <c r="R53">
         <v>0</v>
@@ -10033,7 +10037,7 @@
       </c>
       <c r="Y53">
         <f t="shared" si="0"/>
-        <v>7.6923076923076919E-3</v>
+        <v>5.1282051282051282E-3</v>
       </c>
     </row>
     <row r="54" spans="1:25" x14ac:dyDescent="0.25">
@@ -10086,8 +10090,8 @@
         <v>0</v>
       </c>
       <c r="Q54">
-        <f t="shared" si="1"/>
-        <v>7.6923076923076919E-3</v>
+        <f t="shared" si="2"/>
+        <v>5.1282051282051282E-3</v>
       </c>
       <c r="R54">
         <v>0</v>
@@ -10108,11 +10112,11 @@
         <v>0</v>
       </c>
       <c r="X54">
-        <v>0.2</v>
+        <v>0.9</v>
       </c>
       <c r="Y54">
         <f t="shared" si="0"/>
-        <v>0.2076923076923077</v>
+        <v>0.90512820512820513</v>
       </c>
     </row>
     <row r="55" spans="1:25" x14ac:dyDescent="0.25">
@@ -10165,8 +10169,8 @@
         <v>0</v>
       </c>
       <c r="Q55">
-        <f t="shared" si="1"/>
-        <v>7.6923076923076919E-3</v>
+        <f t="shared" si="2"/>
+        <v>5.1282051282051282E-3</v>
       </c>
       <c r="R55">
         <v>0</v>
@@ -10191,7 +10195,7 @@
       </c>
       <c r="Y55">
         <f t="shared" si="0"/>
-        <v>7.6923076923076919E-3</v>
+        <v>5.1282051282051282E-3</v>
       </c>
     </row>
     <row r="56" spans="1:25" x14ac:dyDescent="0.25">
@@ -10244,8 +10248,8 @@
         <v>0</v>
       </c>
       <c r="Q56">
-        <f t="shared" si="1"/>
-        <v>7.6923076923076919E-3</v>
+        <f t="shared" si="2"/>
+        <v>5.1282051282051282E-3</v>
       </c>
       <c r="R56">
         <v>0</v>
@@ -10270,7 +10274,7 @@
       </c>
       <c r="Y56">
         <f t="shared" si="0"/>
-        <v>7.6923076923076919E-3</v>
+        <v>5.1282051282051282E-3</v>
       </c>
     </row>
     <row r="57" spans="1:25" x14ac:dyDescent="0.25">
@@ -10323,8 +10327,8 @@
         <v>0</v>
       </c>
       <c r="Q57">
-        <f t="shared" si="1"/>
-        <v>7.6923076923076919E-3</v>
+        <f t="shared" si="2"/>
+        <v>5.1282051282051282E-3</v>
       </c>
       <c r="R57">
         <v>0</v>
@@ -10349,7 +10353,7 @@
       </c>
       <c r="Y57">
         <f t="shared" si="0"/>
-        <v>7.6923076923076919E-3</v>
+        <v>5.1282051282051282E-3</v>
       </c>
     </row>
     <row r="58" spans="1:25" x14ac:dyDescent="0.25">
@@ -10402,8 +10406,8 @@
         <v>0</v>
       </c>
       <c r="Q58">
-        <f t="shared" si="1"/>
-        <v>7.6923076923076919E-3</v>
+        <f t="shared" si="2"/>
+        <v>5.1282051282051282E-3</v>
       </c>
       <c r="R58">
         <v>0</v>
@@ -10424,11 +10428,11 @@
         <v>0</v>
       </c>
       <c r="X58">
-        <v>0</v>
+        <v>0.1</v>
       </c>
       <c r="Y58">
         <f t="shared" si="0"/>
-        <v>7.6923076923076919E-3</v>
+        <v>0.10512820512820513</v>
       </c>
     </row>
     <row r="59" spans="1:25" x14ac:dyDescent="0.25">
@@ -10439,7 +10443,7 @@
         <v>0</v>
       </c>
       <c r="C59">
-        <v>0</v>
+        <v>0.1</v>
       </c>
       <c r="D59">
         <v>0</v>
@@ -10481,8 +10485,8 @@
         <v>0</v>
       </c>
       <c r="Q59">
-        <f t="shared" si="1"/>
-        <v>7.6923076923076919E-3</v>
+        <f t="shared" si="2"/>
+        <v>5.1282051282051282E-3</v>
       </c>
       <c r="R59">
         <v>0</v>
@@ -10507,7 +10511,7 @@
       </c>
       <c r="Y59">
         <f t="shared" si="0"/>
-        <v>7.6923076923076919E-3</v>
+        <v>0.10512820512820513</v>
       </c>
     </row>
     <row r="60" spans="1:25" x14ac:dyDescent="0.25">
@@ -10560,8 +10564,8 @@
         <v>0</v>
       </c>
       <c r="Q60">
-        <f t="shared" si="1"/>
-        <v>7.6923076923076919E-3</v>
+        <f t="shared" si="2"/>
+        <v>5.1282051282051282E-3</v>
       </c>
       <c r="R60">
         <v>0</v>
@@ -10586,7 +10590,7 @@
       </c>
       <c r="Y60">
         <f t="shared" si="0"/>
-        <v>7.6923076923076919E-3</v>
+        <v>5.1282051282051282E-3</v>
       </c>
     </row>
     <row r="61" spans="1:25" x14ac:dyDescent="0.25">
@@ -10672,77 +10676,77 @@
         <v>78</v>
       </c>
       <c r="B62">
-        <v>0.9</v>
+        <v>0.8</v>
       </c>
       <c r="C62">
+        <v>0.6</v>
+      </c>
+      <c r="D62">
+        <v>1</v>
+      </c>
+      <c r="E62">
         <v>0.7</v>
       </c>
-      <c r="D62">
-        <v>0.9</v>
-      </c>
-      <c r="E62">
+      <c r="F62">
+        <v>0.6</v>
+      </c>
+      <c r="G62">
+        <v>0.6</v>
+      </c>
+      <c r="H62">
+        <v>0</v>
+      </c>
+      <c r="I62">
+        <v>0</v>
+      </c>
+      <c r="J62">
+        <v>0.85</v>
+      </c>
+      <c r="K62">
+        <v>0.95</v>
+      </c>
+      <c r="L62">
+        <v>0.75</v>
+      </c>
+      <c r="M62">
+        <v>0</v>
+      </c>
+      <c r="N62">
+        <v>1E-3</v>
+      </c>
+      <c r="O62">
+        <v>1E-3</v>
+      </c>
+      <c r="P62">
+        <v>0.45</v>
+      </c>
+      <c r="Q62">
         <v>0.8</v>
       </c>
-      <c r="F62">
-        <v>0.9</v>
-      </c>
-      <c r="G62">
-        <v>0.9</v>
-      </c>
-      <c r="H62">
-        <v>0.1</v>
-      </c>
-      <c r="I62">
-        <v>0</v>
-      </c>
-      <c r="J62">
-        <v>0.9</v>
-      </c>
-      <c r="K62">
+      <c r="R62">
+        <v>0.5</v>
+      </c>
+      <c r="S62">
         <v>0.8</v>
       </c>
-      <c r="L62">
-        <v>0.8</v>
-      </c>
-      <c r="M62">
-        <v>0.6</v>
-      </c>
-      <c r="N62">
-        <v>0.2</v>
-      </c>
-      <c r="O62">
-        <v>0</v>
-      </c>
-      <c r="P62">
-        <v>0.4</v>
-      </c>
-      <c r="Q62">
+      <c r="T62">
+        <v>0</v>
+      </c>
+      <c r="U62">
         <v>0.7</v>
       </c>
-      <c r="R62">
-        <v>0.1</v>
-      </c>
-      <c r="S62">
-        <v>0.4</v>
-      </c>
-      <c r="T62">
-        <v>0</v>
-      </c>
-      <c r="U62">
-        <v>0.4</v>
-      </c>
       <c r="V62">
-        <v>0.8</v>
+        <v>0.96</v>
       </c>
       <c r="W62">
         <v>1</v>
       </c>
       <c r="X62">
-        <v>0.6</v>
+        <v>0</v>
       </c>
       <c r="Y62">
         <f t="shared" si="0"/>
-        <v>12.9</v>
+        <v>12.062000000000001</v>
       </c>
     </row>
     <row r="63" spans="1:25" x14ac:dyDescent="0.25">
@@ -10751,90 +10755,91 @@
         <v>1</v>
       </c>
       <c r="C63">
-        <f t="shared" ref="C63:X63" si="2">SUM(C2:C62)</f>
+        <f t="shared" ref="C63:X63" si="3">SUM(C2:C62)</f>
         <v>1</v>
       </c>
       <c r="D63">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>1</v>
       </c>
       <c r="E63">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>1</v>
       </c>
       <c r="F63">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>1</v>
       </c>
       <c r="G63">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>1</v>
       </c>
       <c r="H63">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>1</v>
       </c>
       <c r="I63">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>1</v>
       </c>
       <c r="J63">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>1</v>
       </c>
       <c r="K63">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>1</v>
       </c>
       <c r="L63">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>1</v>
       </c>
       <c r="M63">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>1</v>
       </c>
       <c r="N63">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>1</v>
       </c>
       <c r="O63">
-        <v>1E-3</v>
+        <f t="shared" si="3"/>
+        <v>1</v>
       </c>
       <c r="P63">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>1</v>
       </c>
       <c r="Q63">
-        <f t="shared" si="2"/>
-        <v>0.99999999999999978</v>
+        <f t="shared" si="3"/>
+        <v>1.0000000000000002</v>
       </c>
       <c r="R63">
-        <f t="shared" si="2"/>
-        <v>0.99999999999999989</v>
+        <f t="shared" si="3"/>
+        <v>1</v>
       </c>
       <c r="S63">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>1</v>
       </c>
       <c r="T63">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>1</v>
       </c>
       <c r="U63">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>1</v>
       </c>
       <c r="V63">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>1</v>
       </c>
       <c r="W63">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>1</v>
       </c>
       <c r="X63">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>1</v>
       </c>
     </row>

</xml_diff>